<commit_message>
set font on copycat example
</commit_message>
<xml_diff>
--- a/Copycat/test2-libre.xlsx
+++ b/Copycat/test2-libre.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">S1 A1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">S1 B1</t>
   </si>
@@ -113,7 +110,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFF10D0C"/>
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
@@ -123,7 +120,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFF10D0C"/>
         <rFont val="돋움"/>
         <family val="2"/>
         <charset val="129"/>
@@ -139,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -167,6 +164,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -178,13 +181,46 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFF10D0C"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFF10D0C"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,7 +266,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,6 +307,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFF10D0C"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -254,8 +378,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -263,25 +387,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="13.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -304,7 +426,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,32 +435,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D4" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -360,8 +482,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -369,27 +491,27 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="13.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="9" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set col/width of cell
</commit_message>
<xml_diff>
--- a/Copycat/test2-libre.xlsx
+++ b/Copycat/test2-libre.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" state="visible" r:id="rId2"/>
@@ -136,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -175,6 +175,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFCE181E"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2A6099"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -184,13 +198,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00A933"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE181E"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -271,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,15 +291,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,7 +315,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,7 +323,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,18 +331,18 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -353,7 +368,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -400,13 +415,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="13.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,16 +432,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="130.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -447,7 +464,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -465,10 +482,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -476,12 +493,12 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -514,25 +531,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>